<commit_message>
add some styles for fun
</commit_message>
<xml_diff>
--- a/heading_template.xlsx
+++ b/heading_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23325" windowHeight="9795" tabRatio="500"/>
+    <workbookView windowWidth="24000" windowHeight="9795" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Invoice" sheetId="1" r:id="rId1"/>
@@ -217,11 +217,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -237,9 +237,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,16 +264,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,23 +303,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,20 +324,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -342,14 +341,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -359,6 +350,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,14 +379,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,7 +402,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,19 +486,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,25 +498,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,121 +582,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,28 +596,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,15 +625,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,50 +668,67 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -737,97 +737,97 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1157,7 +1157,7 @@
   <dimension ref="A1:BM1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14.25"/>
@@ -1432,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>

</xml_diff>